<commit_message>
JE BOt update-- without sap upload component
</commit_message>
<xml_diff>
--- a/My Docs/JE Docs/2020 Transfer from Accum to Equivest workbook.xlsx
+++ b/My Docs/JE Docs/2020 Transfer from Accum to Equivest workbook.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20348"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayadav\Documents\Automation Anywhere Files\Automation Anywhere\My Docs\JE Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969ED39E-86B3-4AE1-8D0D-CDA7AD6E041D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8475" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8475" tabRatio="754"/>
   </bookViews>
   <sheets>
     <sheet name="April" sheetId="14" r:id="rId1"/>
@@ -197,7 +196,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1263,247 +1262,247 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="241">
-    <cellStyle name="20% - Accent1 2" xfId="159" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent1 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="160" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="161" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent3 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="162" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - Accent4 3" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="163" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - Accent5 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="164" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - Accent6 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="165" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="40% - Accent1 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="166" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="40% - Accent2 3" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="167" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="40% - Accent3 3" xfId="16" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="168" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="40% - Accent4 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="169" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="40% - Accent5 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="170" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="40% - Accent6 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="171" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="60% - Accent1 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="172" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="60% - Accent2 3" xfId="21" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="173" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="60% - Accent3 3" xfId="22" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="174" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="60% - Accent4 3" xfId="23" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="175" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="60% - Accent5 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="176" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="60% - Accent6 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Accent1 2" xfId="177" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Accent1 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Accent2 2" xfId="178" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Accent2 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Accent3 2" xfId="179" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Accent3 3" xfId="28" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Accent4 2" xfId="180" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Accent4 3" xfId="29" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Accent5 2" xfId="181" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Accent5 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Accent6 2" xfId="182" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Accent6 3" xfId="31" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Bad 2" xfId="183" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Bad 3" xfId="32" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Calculation 2" xfId="184" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Calculation 3" xfId="33" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Check Cell 2" xfId="185" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Check Cell 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Comma 2 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Comma 2 2 2" xfId="186" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Comma 2 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Comma 3" xfId="5" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Comma 3 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Comma 3 3" xfId="187" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Comma 3 4" xfId="37" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Comma 4" xfId="39" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Comma 5" xfId="237" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Currency 2 2" xfId="239" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Currency 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Currency 3 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="188" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Explanatory Text 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Good 2" xfId="189" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Good 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Heading 1 2" xfId="190" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Heading 1 3" xfId="43" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Heading 2 2" xfId="191" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Heading 2 3" xfId="44" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Heading 3 2" xfId="192" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Heading 3 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Heading 4 2" xfId="193" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Heading 4 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Input 2" xfId="194" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Input 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="195" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Linked Cell 3" xfId="48" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Neutral 2" xfId="196" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Neutral 3" xfId="49" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="159"/>
+    <cellStyle name="20% - Accent1 3" xfId="8"/>
+    <cellStyle name="20% - Accent2 2" xfId="160"/>
+    <cellStyle name="20% - Accent2 3" xfId="9"/>
+    <cellStyle name="20% - Accent3 2" xfId="161"/>
+    <cellStyle name="20% - Accent3 3" xfId="10"/>
+    <cellStyle name="20% - Accent4 2" xfId="162"/>
+    <cellStyle name="20% - Accent4 3" xfId="11"/>
+    <cellStyle name="20% - Accent5 2" xfId="163"/>
+    <cellStyle name="20% - Accent5 3" xfId="12"/>
+    <cellStyle name="20% - Accent6 2" xfId="164"/>
+    <cellStyle name="20% - Accent6 3" xfId="13"/>
+    <cellStyle name="40% - Accent1 2" xfId="165"/>
+    <cellStyle name="40% - Accent1 3" xfId="14"/>
+    <cellStyle name="40% - Accent2 2" xfId="166"/>
+    <cellStyle name="40% - Accent2 3" xfId="15"/>
+    <cellStyle name="40% - Accent3 2" xfId="167"/>
+    <cellStyle name="40% - Accent3 3" xfId="16"/>
+    <cellStyle name="40% - Accent4 2" xfId="168"/>
+    <cellStyle name="40% - Accent4 3" xfId="17"/>
+    <cellStyle name="40% - Accent5 2" xfId="169"/>
+    <cellStyle name="40% - Accent5 3" xfId="18"/>
+    <cellStyle name="40% - Accent6 2" xfId="170"/>
+    <cellStyle name="40% - Accent6 3" xfId="19"/>
+    <cellStyle name="60% - Accent1 2" xfId="171"/>
+    <cellStyle name="60% - Accent1 3" xfId="20"/>
+    <cellStyle name="60% - Accent2 2" xfId="172"/>
+    <cellStyle name="60% - Accent2 3" xfId="21"/>
+    <cellStyle name="60% - Accent3 2" xfId="173"/>
+    <cellStyle name="60% - Accent3 3" xfId="22"/>
+    <cellStyle name="60% - Accent4 2" xfId="174"/>
+    <cellStyle name="60% - Accent4 3" xfId="23"/>
+    <cellStyle name="60% - Accent5 2" xfId="175"/>
+    <cellStyle name="60% - Accent5 3" xfId="24"/>
+    <cellStyle name="60% - Accent6 2" xfId="176"/>
+    <cellStyle name="60% - Accent6 3" xfId="25"/>
+    <cellStyle name="Accent1 2" xfId="177"/>
+    <cellStyle name="Accent1 3" xfId="26"/>
+    <cellStyle name="Accent2 2" xfId="178"/>
+    <cellStyle name="Accent2 3" xfId="27"/>
+    <cellStyle name="Accent3 2" xfId="179"/>
+    <cellStyle name="Accent3 3" xfId="28"/>
+    <cellStyle name="Accent4 2" xfId="180"/>
+    <cellStyle name="Accent4 3" xfId="29"/>
+    <cellStyle name="Accent5 2" xfId="181"/>
+    <cellStyle name="Accent5 3" xfId="30"/>
+    <cellStyle name="Accent6 2" xfId="182"/>
+    <cellStyle name="Accent6 3" xfId="31"/>
+    <cellStyle name="Bad 2" xfId="183"/>
+    <cellStyle name="Bad 3" xfId="32"/>
+    <cellStyle name="Calculation 2" xfId="184"/>
+    <cellStyle name="Calculation 3" xfId="33"/>
+    <cellStyle name="Check Cell 2" xfId="185"/>
+    <cellStyle name="Check Cell 3" xfId="34"/>
+    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2 2" xfId="36"/>
+    <cellStyle name="Comma 2 2 2" xfId="186"/>
+    <cellStyle name="Comma 2 3" xfId="35"/>
+    <cellStyle name="Comma 3" xfId="5"/>
+    <cellStyle name="Comma 3 2" xfId="38"/>
+    <cellStyle name="Comma 3 3" xfId="187"/>
+    <cellStyle name="Comma 3 4" xfId="37"/>
+    <cellStyle name="Comma 4" xfId="39"/>
+    <cellStyle name="Comma 5" xfId="237"/>
+    <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Currency 2 2" xfId="239"/>
+    <cellStyle name="Currency 3" xfId="6"/>
+    <cellStyle name="Currency 3 2" xfId="40"/>
+    <cellStyle name="Explanatory Text 2" xfId="188"/>
+    <cellStyle name="Explanatory Text 3" xfId="41"/>
+    <cellStyle name="Good 2" xfId="189"/>
+    <cellStyle name="Good 3" xfId="42"/>
+    <cellStyle name="Heading 1 2" xfId="190"/>
+    <cellStyle name="Heading 1 3" xfId="43"/>
+    <cellStyle name="Heading 2 2" xfId="191"/>
+    <cellStyle name="Heading 2 3" xfId="44"/>
+    <cellStyle name="Heading 3 2" xfId="192"/>
+    <cellStyle name="Heading 3 3" xfId="45"/>
+    <cellStyle name="Heading 4 2" xfId="193"/>
+    <cellStyle name="Heading 4 3" xfId="46"/>
+    <cellStyle name="Input 2" xfId="194"/>
+    <cellStyle name="Input 3" xfId="47"/>
+    <cellStyle name="Linked Cell 2" xfId="195"/>
+    <cellStyle name="Linked Cell 3" xfId="48"/>
+    <cellStyle name="Neutral 2" xfId="196"/>
+    <cellStyle name="Neutral 3" xfId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 2 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="197" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 2 3" xfId="50" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 3 3" xfId="240" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4" xfId="53" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 5" xfId="54" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 5 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 5_04-30" xfId="56" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 6" xfId="158" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 7" xfId="157" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 8" xfId="7" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 9" xfId="238" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Note 2" xfId="198" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Note 3" xfId="57" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Output 2" xfId="199" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Output 3" xfId="58" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="PSChar" xfId="59" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="PSChar 10" xfId="60" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="PSChar 10 2" xfId="200" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="PSChar 11" xfId="61" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="PSChar 11 2" xfId="201" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="PSChar 12" xfId="62" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="PSChar 12 2" xfId="202" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="PSChar 13" xfId="63" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="PSChar 13 2" xfId="203" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="PSChar 14" xfId="64" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="PSChar 14 2" xfId="204" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="PSChar 15" xfId="65" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="PSChar 15 2" xfId="205" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="PSChar 16" xfId="66" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
-    <cellStyle name="PSChar 16 2" xfId="206" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
-    <cellStyle name="PSChar 2" xfId="67" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="PSChar 3" xfId="68" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="PSChar 4" xfId="69" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="PSChar 5" xfId="70" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="PSChar 5 2" xfId="71" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="PSChar 6" xfId="72" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="PSChar 6 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="PSChar 7" xfId="74" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="PSChar 7 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="PSChar 8" xfId="76" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="PSChar 8 2" xfId="77" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="PSChar 9" xfId="78" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="PSChar 9 2" xfId="79" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="PSDate" xfId="80" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="PSDate 10" xfId="81" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="PSDate 10 2" xfId="207" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="PSDate 11" xfId="82" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="PSDate 11 2" xfId="208" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="PSDate 12" xfId="83" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="PSDate 12 2" xfId="209" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="PSDate 13" xfId="84" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="PSDate 13 2" xfId="210" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="PSDate 14" xfId="85" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="PSDate 14 2" xfId="211" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="PSDate 15" xfId="86" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="PSDate 15 2" xfId="212" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="PSDate 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="PSDate 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="PSDate 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="PSDate 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="PSDate 5" xfId="91" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="PSDate 5 2" xfId="92" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="PSDate 6" xfId="93" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
-    <cellStyle name="PSDate 6 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
-    <cellStyle name="PSDate 7" xfId="95" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
-    <cellStyle name="PSDate 7 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
-    <cellStyle name="PSDate 8" xfId="97" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
-    <cellStyle name="PSDate 8 2" xfId="98" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
-    <cellStyle name="PSDate 9" xfId="99" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
-    <cellStyle name="PSDate 9 2" xfId="213" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
-    <cellStyle name="PSDec" xfId="100" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
-    <cellStyle name="PSDec 10" xfId="101" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
-    <cellStyle name="PSDec 10 2" xfId="214" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
-    <cellStyle name="PSDec 11" xfId="102" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
-    <cellStyle name="PSDec 11 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
-    <cellStyle name="PSDec 12" xfId="103" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
-    <cellStyle name="PSDec 12 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
-    <cellStyle name="PSDec 13" xfId="104" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
-    <cellStyle name="PSDec 13 2" xfId="217" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
-    <cellStyle name="PSDec 14" xfId="105" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
-    <cellStyle name="PSDec 14 2" xfId="218" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
-    <cellStyle name="PSDec 15" xfId="106" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
-    <cellStyle name="PSDec 15 2" xfId="219" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
-    <cellStyle name="PSDec 16" xfId="107" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
-    <cellStyle name="PSDec 16 2" xfId="220" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
-    <cellStyle name="PSDec 2" xfId="108" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
-    <cellStyle name="PSDec 3" xfId="109" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
-    <cellStyle name="PSDec 4" xfId="110" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
-    <cellStyle name="PSDec 5" xfId="111" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
-    <cellStyle name="PSDec 5 2" xfId="112" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
-    <cellStyle name="PSDec 6" xfId="113" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
-    <cellStyle name="PSDec 6 2" xfId="114" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
-    <cellStyle name="PSDec 7" xfId="115" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
-    <cellStyle name="PSDec 7 2" xfId="116" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
-    <cellStyle name="PSDec 8" xfId="117" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="PSDec 8 2" xfId="118" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
-    <cellStyle name="PSDec 9" xfId="119" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
-    <cellStyle name="PSDec 9 2" xfId="120" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
-    <cellStyle name="PSHeading" xfId="121" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
-    <cellStyle name="PSHeading 2" xfId="122" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
-    <cellStyle name="PSHeading 2 2" xfId="221" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
-    <cellStyle name="PSHeading 3" xfId="123" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
-    <cellStyle name="PSHeading 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
-    <cellStyle name="PSHeading 3 2 2" xfId="222" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
-    <cellStyle name="PSHeading 3 3" xfId="125" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
-    <cellStyle name="PSHeading 3 3 2" xfId="223" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
-    <cellStyle name="PSHeading 3 4" xfId="126" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="PSHeading 3 4 2" xfId="224" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
-    <cellStyle name="PSHeading 3 5" xfId="127" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
-    <cellStyle name="PSHeading 3 5 2" xfId="225" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
-    <cellStyle name="PSHeading 3 6" xfId="128" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
-    <cellStyle name="PSHeading 3 6 2" xfId="226" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
-    <cellStyle name="PSHeading 3 7" xfId="129" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
-    <cellStyle name="PSHeading 3 7 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
-    <cellStyle name="PSHeading 3_03-31 final (2)" xfId="130" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
-    <cellStyle name="PSHeading 4" xfId="131" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
-    <cellStyle name="PSHeading 4 2" xfId="228" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
-    <cellStyle name="PSHeading 5" xfId="132" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
-    <cellStyle name="PSHeading 5 2" xfId="229" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
-    <cellStyle name="PSHeading 6" xfId="133" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
-    <cellStyle name="PSHeading 6 2" xfId="230" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
-    <cellStyle name="PSHeading 7" xfId="134" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
-    <cellStyle name="PSHeading 7 2" xfId="231" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
-    <cellStyle name="PSHeading 8" xfId="135" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
-    <cellStyle name="PSHeading 8 2" xfId="232" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="PSHeading 9" xfId="136" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
-    <cellStyle name="PSHeading 9 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
-    <cellStyle name="PSHeading_03-31 final (2)" xfId="137" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
-    <cellStyle name="PSInt" xfId="138" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
-    <cellStyle name="PSInt 2" xfId="139" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
-    <cellStyle name="PSInt 3" xfId="140" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
-    <cellStyle name="PSInt 4" xfId="141" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
-    <cellStyle name="PSInt 5" xfId="142" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
-    <cellStyle name="PSInt 6" xfId="143" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
-    <cellStyle name="PSInt 7" xfId="144" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
-    <cellStyle name="PSInt 8" xfId="145" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
-    <cellStyle name="PSSpacer" xfId="146" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
-    <cellStyle name="PSSpacer 2" xfId="147" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
-    <cellStyle name="PSSpacer 3" xfId="148" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
-    <cellStyle name="PSSpacer 4" xfId="149" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
-    <cellStyle name="PSSpacer 5" xfId="150" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
-    <cellStyle name="PSSpacer 6" xfId="151" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
-    <cellStyle name="PSSpacer 7" xfId="152" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
-    <cellStyle name="PSSpacer 8" xfId="153" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
-    <cellStyle name="Title 2" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
-    <cellStyle name="Title 3" xfId="154" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
-    <cellStyle name="Total 2" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
-    <cellStyle name="Total 3" xfId="155" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
-    <cellStyle name="Warning Text 2" xfId="236" xr:uid="{00000000-0005-0000-0000-0000F0000000}"/>
-    <cellStyle name="Warning Text 3" xfId="156" xr:uid="{00000000-0005-0000-0000-0000F1000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="51"/>
+    <cellStyle name="Normal 2 2 2" xfId="197"/>
+    <cellStyle name="Normal 2 3" xfId="50"/>
+    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 3 2" xfId="52"/>
+    <cellStyle name="Normal 3 3" xfId="240"/>
+    <cellStyle name="Normal 4" xfId="53"/>
+    <cellStyle name="Normal 5" xfId="54"/>
+    <cellStyle name="Normal 5 2" xfId="55"/>
+    <cellStyle name="Normal 5_04-30" xfId="56"/>
+    <cellStyle name="Normal 6" xfId="158"/>
+    <cellStyle name="Normal 7" xfId="157"/>
+    <cellStyle name="Normal 8" xfId="7"/>
+    <cellStyle name="Normal 9" xfId="238"/>
+    <cellStyle name="Note 2" xfId="198"/>
+    <cellStyle name="Note 3" xfId="57"/>
+    <cellStyle name="Output 2" xfId="199"/>
+    <cellStyle name="Output 3" xfId="58"/>
+    <cellStyle name="PSChar" xfId="59"/>
+    <cellStyle name="PSChar 10" xfId="60"/>
+    <cellStyle name="PSChar 10 2" xfId="200"/>
+    <cellStyle name="PSChar 11" xfId="61"/>
+    <cellStyle name="PSChar 11 2" xfId="201"/>
+    <cellStyle name="PSChar 12" xfId="62"/>
+    <cellStyle name="PSChar 12 2" xfId="202"/>
+    <cellStyle name="PSChar 13" xfId="63"/>
+    <cellStyle name="PSChar 13 2" xfId="203"/>
+    <cellStyle name="PSChar 14" xfId="64"/>
+    <cellStyle name="PSChar 14 2" xfId="204"/>
+    <cellStyle name="PSChar 15" xfId="65"/>
+    <cellStyle name="PSChar 15 2" xfId="205"/>
+    <cellStyle name="PSChar 16" xfId="66"/>
+    <cellStyle name="PSChar 16 2" xfId="206"/>
+    <cellStyle name="PSChar 2" xfId="67"/>
+    <cellStyle name="PSChar 3" xfId="68"/>
+    <cellStyle name="PSChar 4" xfId="69"/>
+    <cellStyle name="PSChar 5" xfId="70"/>
+    <cellStyle name="PSChar 5 2" xfId="71"/>
+    <cellStyle name="PSChar 6" xfId="72"/>
+    <cellStyle name="PSChar 6 2" xfId="73"/>
+    <cellStyle name="PSChar 7" xfId="74"/>
+    <cellStyle name="PSChar 7 2" xfId="75"/>
+    <cellStyle name="PSChar 8" xfId="76"/>
+    <cellStyle name="PSChar 8 2" xfId="77"/>
+    <cellStyle name="PSChar 9" xfId="78"/>
+    <cellStyle name="PSChar 9 2" xfId="79"/>
+    <cellStyle name="PSDate" xfId="80"/>
+    <cellStyle name="PSDate 10" xfId="81"/>
+    <cellStyle name="PSDate 10 2" xfId="207"/>
+    <cellStyle name="PSDate 11" xfId="82"/>
+    <cellStyle name="PSDate 11 2" xfId="208"/>
+    <cellStyle name="PSDate 12" xfId="83"/>
+    <cellStyle name="PSDate 12 2" xfId="209"/>
+    <cellStyle name="PSDate 13" xfId="84"/>
+    <cellStyle name="PSDate 13 2" xfId="210"/>
+    <cellStyle name="PSDate 14" xfId="85"/>
+    <cellStyle name="PSDate 14 2" xfId="211"/>
+    <cellStyle name="PSDate 15" xfId="86"/>
+    <cellStyle name="PSDate 15 2" xfId="212"/>
+    <cellStyle name="PSDate 2" xfId="87"/>
+    <cellStyle name="PSDate 3" xfId="88"/>
+    <cellStyle name="PSDate 4" xfId="89"/>
+    <cellStyle name="PSDate 4 2" xfId="90"/>
+    <cellStyle name="PSDate 5" xfId="91"/>
+    <cellStyle name="PSDate 5 2" xfId="92"/>
+    <cellStyle name="PSDate 6" xfId="93"/>
+    <cellStyle name="PSDate 6 2" xfId="94"/>
+    <cellStyle name="PSDate 7" xfId="95"/>
+    <cellStyle name="PSDate 7 2" xfId="96"/>
+    <cellStyle name="PSDate 8" xfId="97"/>
+    <cellStyle name="PSDate 8 2" xfId="98"/>
+    <cellStyle name="PSDate 9" xfId="99"/>
+    <cellStyle name="PSDate 9 2" xfId="213"/>
+    <cellStyle name="PSDec" xfId="100"/>
+    <cellStyle name="PSDec 10" xfId="101"/>
+    <cellStyle name="PSDec 10 2" xfId="214"/>
+    <cellStyle name="PSDec 11" xfId="102"/>
+    <cellStyle name="PSDec 11 2" xfId="215"/>
+    <cellStyle name="PSDec 12" xfId="103"/>
+    <cellStyle name="PSDec 12 2" xfId="216"/>
+    <cellStyle name="PSDec 13" xfId="104"/>
+    <cellStyle name="PSDec 13 2" xfId="217"/>
+    <cellStyle name="PSDec 14" xfId="105"/>
+    <cellStyle name="PSDec 14 2" xfId="218"/>
+    <cellStyle name="PSDec 15" xfId="106"/>
+    <cellStyle name="PSDec 15 2" xfId="219"/>
+    <cellStyle name="PSDec 16" xfId="107"/>
+    <cellStyle name="PSDec 16 2" xfId="220"/>
+    <cellStyle name="PSDec 2" xfId="108"/>
+    <cellStyle name="PSDec 3" xfId="109"/>
+    <cellStyle name="PSDec 4" xfId="110"/>
+    <cellStyle name="PSDec 5" xfId="111"/>
+    <cellStyle name="PSDec 5 2" xfId="112"/>
+    <cellStyle name="PSDec 6" xfId="113"/>
+    <cellStyle name="PSDec 6 2" xfId="114"/>
+    <cellStyle name="PSDec 7" xfId="115"/>
+    <cellStyle name="PSDec 7 2" xfId="116"/>
+    <cellStyle name="PSDec 8" xfId="117"/>
+    <cellStyle name="PSDec 8 2" xfId="118"/>
+    <cellStyle name="PSDec 9" xfId="119"/>
+    <cellStyle name="PSDec 9 2" xfId="120"/>
+    <cellStyle name="PSHeading" xfId="121"/>
+    <cellStyle name="PSHeading 2" xfId="122"/>
+    <cellStyle name="PSHeading 2 2" xfId="221"/>
+    <cellStyle name="PSHeading 3" xfId="123"/>
+    <cellStyle name="PSHeading 3 2" xfId="124"/>
+    <cellStyle name="PSHeading 3 2 2" xfId="222"/>
+    <cellStyle name="PSHeading 3 3" xfId="125"/>
+    <cellStyle name="PSHeading 3 3 2" xfId="223"/>
+    <cellStyle name="PSHeading 3 4" xfId="126"/>
+    <cellStyle name="PSHeading 3 4 2" xfId="224"/>
+    <cellStyle name="PSHeading 3 5" xfId="127"/>
+    <cellStyle name="PSHeading 3 5 2" xfId="225"/>
+    <cellStyle name="PSHeading 3 6" xfId="128"/>
+    <cellStyle name="PSHeading 3 6 2" xfId="226"/>
+    <cellStyle name="PSHeading 3 7" xfId="129"/>
+    <cellStyle name="PSHeading 3 7 2" xfId="227"/>
+    <cellStyle name="PSHeading 3_03-31 final (2)" xfId="130"/>
+    <cellStyle name="PSHeading 4" xfId="131"/>
+    <cellStyle name="PSHeading 4 2" xfId="228"/>
+    <cellStyle name="PSHeading 5" xfId="132"/>
+    <cellStyle name="PSHeading 5 2" xfId="229"/>
+    <cellStyle name="PSHeading 6" xfId="133"/>
+    <cellStyle name="PSHeading 6 2" xfId="230"/>
+    <cellStyle name="PSHeading 7" xfId="134"/>
+    <cellStyle name="PSHeading 7 2" xfId="231"/>
+    <cellStyle name="PSHeading 8" xfId="135"/>
+    <cellStyle name="PSHeading 8 2" xfId="232"/>
+    <cellStyle name="PSHeading 9" xfId="136"/>
+    <cellStyle name="PSHeading 9 2" xfId="233"/>
+    <cellStyle name="PSHeading_03-31 final (2)" xfId="137"/>
+    <cellStyle name="PSInt" xfId="138"/>
+    <cellStyle name="PSInt 2" xfId="139"/>
+    <cellStyle name="PSInt 3" xfId="140"/>
+    <cellStyle name="PSInt 4" xfId="141"/>
+    <cellStyle name="PSInt 5" xfId="142"/>
+    <cellStyle name="PSInt 6" xfId="143"/>
+    <cellStyle name="PSInt 7" xfId="144"/>
+    <cellStyle name="PSInt 8" xfId="145"/>
+    <cellStyle name="PSSpacer" xfId="146"/>
+    <cellStyle name="PSSpacer 2" xfId="147"/>
+    <cellStyle name="PSSpacer 3" xfId="148"/>
+    <cellStyle name="PSSpacer 4" xfId="149"/>
+    <cellStyle name="PSSpacer 5" xfId="150"/>
+    <cellStyle name="PSSpacer 6" xfId="151"/>
+    <cellStyle name="PSSpacer 7" xfId="152"/>
+    <cellStyle name="PSSpacer 8" xfId="153"/>
+    <cellStyle name="Title 2" xfId="234"/>
+    <cellStyle name="Title 3" xfId="154"/>
+    <cellStyle name="Total 2" xfId="235"/>
+    <cellStyle name="Total 3" xfId="155"/>
+    <cellStyle name="Warning Text 2" xfId="236"/>
+    <cellStyle name="Warning Text 3" xfId="156"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1594,23 +1593,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1646,23 +1628,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1838,10 +1803,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>